<commit_message>
xuất phiếu đóng phạt (PDF)
</commit_message>
<xml_diff>
--- a/Library_API/Upload/importfile.xlsx
+++ b/Library_API/Upload/importfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK2 2023-2024\TN408 NienLuan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9992C5-C72F-41CE-972A-A581539258E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46F71BE-38D3-489B-8107-2489007F5254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80549B35-C4EB-4A7C-B8D2-F0AF8A9BC7A4}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
-  <si>
-    <t>mon</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -72,37 +69,22 @@
     <t>Quyen</t>
   </si>
   <si>
-    <t>nam</t>
-  </si>
-  <si>
-    <t>man</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>thanh</t>
-  </si>
-  <si>
-    <t>Trần Văn Mon</t>
-  </si>
-  <si>
-    <t>Trần Văn Man</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trần Thị Thanh Thanh </t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>mmtttt1404@gmail.com</t>
+    <t>duy</t>
+  </si>
+  <si>
+    <t>Trương Văn Duy</t>
+  </si>
+  <si>
+    <t>VL</t>
+  </si>
+  <si>
+    <t>duyb2005667@student.ctu.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -280,10 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,7 +584,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,42 +593,42 @@
     <col min="5" max="5" width="16.44140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.88671875" style="7" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="10"/>
-    <col min="11" max="11" width="14.44140625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="27.5546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="K1" s="14" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -654,105 +636,51 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>123</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6">
-        <v>37360</v>
+        <v>37446</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H2" s="6">
-        <v>45371</v>
+        <v>45373</v>
       </c>
       <c r="I2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11">
-        <v>123</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="12">
-        <v>41874</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="6">
-        <v>45371</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="H3" s="6"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="11">
-        <v>123</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44754</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="6">
-        <v>45371</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="H4" s="6"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H5"/>
@@ -760,11 +688,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{4FB3DE1D-FEA5-46B2-97ED-EE367E254E1A}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{CDFEBAB7-AE83-4417-92E3-00A580F25A6E}"/>
-    <hyperlink ref="K2" r:id="rId3" xr:uid="{3BBA6F20-EDC2-4EA7-9B6C-CCA8FE22D0A8}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{3BBA6F20-EDC2-4EA7-9B6C-CCA8FE22D0A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cải tiến các góp ý trong niên luận
</commit_message>
<xml_diff>
--- a/Library_API/Upload/importfile.xlsx
+++ b/Library_API/Upload/importfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK2 2023-2024\TN408 NienLuan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46F71BE-38D3-489B-8107-2489007F5254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2000AF-D9FD-495A-B661-CDD026965CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80549B35-C4EB-4A7C-B8D2-F0AF8A9BC7A4}"/>
   </bookViews>
@@ -60,31 +60,31 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Nam</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
     <t>Quyen</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>duy</t>
-  </si>
-  <si>
-    <t>Trương Văn Duy</t>
-  </si>
-  <si>
-    <t>VL</t>
-  </si>
-  <si>
-    <t>duyb2005667@student.ctu.edu.vn</t>
+    <t>02</t>
+  </si>
+  <si>
+    <t>thanhb2005691@student.ctu.edu.vn</t>
+  </si>
+  <si>
+    <t>cam</t>
+  </si>
+  <si>
+    <t>Trương Thị Cam Cam</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Vĩnh Long</t>
   </si>
 </sst>
 </file>
@@ -584,11 +584,13 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.88671875" style="7" customWidth="1"/>
@@ -598,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -625,10 +627,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -647,14 +649,14 @@
       <c r="E2" s="6">
         <v>37446</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="6">
-        <v>45373</v>
+        <v>45403</v>
       </c>
       <c r="I2" s="4" t="b">
         <v>1</v>
@@ -663,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
giao diện thanh toán VNPAY
</commit_message>
<xml_diff>
--- a/Library_API/Upload/importfile.xlsx
+++ b/Library_API/Upload/importfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK2 2023-2024\TN408 NienLuan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK1 2024-2025\CT554 LuanVan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2000AF-D9FD-495A-B661-CDD026965CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769E8FD3-A602-4CA7-921E-9E9195F53BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80549B35-C4EB-4A7C-B8D2-F0AF8A9BC7A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -69,22 +69,100 @@
     <t>Email</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>thanhb2005691@student.ctu.edu.vn</t>
-  </si>
-  <si>
-    <t>cam</t>
-  </si>
-  <si>
-    <t>Trương Thị Cam Cam</t>
-  </si>
-  <si>
-    <t>Nữ</t>
-  </si>
-  <si>
-    <t>Vĩnh Long</t>
+    <t>CCCD</t>
+  </si>
+  <si>
+    <t>SoDienThoai</t>
+  </si>
+  <si>
+    <t>HinhThe</t>
+  </si>
+  <si>
+    <t>apple_user</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>Nguyen Van A</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>apple_user@example.com</t>
+  </si>
+  <si>
+    <t>Ha Noi</t>
+  </si>
+  <si>
+    <t>banana_user</t>
+  </si>
+  <si>
+    <t>pass456</t>
+  </si>
+  <si>
+    <t>Tran Thi B</t>
+  </si>
+  <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>banana_user@example.com</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>cherry_user</t>
+  </si>
+  <si>
+    <t>pass789</t>
+  </si>
+  <si>
+    <t>Le Van C</t>
+  </si>
+  <si>
+    <t>cherry_user@example.com</t>
+  </si>
+  <si>
+    <t>Da Nang</t>
+  </si>
+  <si>
+    <t>grape_user</t>
+  </si>
+  <si>
+    <t>pass321</t>
+  </si>
+  <si>
+    <t>Pham Thi D</t>
+  </si>
+  <si>
+    <t>grape_user@example.com</t>
+  </si>
+  <si>
+    <t>Can Tho</t>
+  </si>
+  <si>
+    <t>mango_user</t>
+  </si>
+  <si>
+    <t>pass654</t>
+  </si>
+  <si>
+    <t>Vu Van E</t>
+  </si>
+  <si>
+    <t>mango_user@example.com</t>
+  </si>
+  <si>
+    <t>Hai Phong</t>
+  </si>
+  <si>
+    <t>ThoiGianSuDung</t>
+  </si>
+  <si>
+    <t>LoaiNguoiDung</t>
   </si>
 </sst>
 </file>
@@ -109,15 +187,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9.6"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,40 +217,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE3E3E3"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFE3E3E3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFE3E3E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE3E3E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE3E3E3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFE3E3E3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFE3E3E3"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -185,30 +237,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFE3E3E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE3E3E3"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFE3E3E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE3E3E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFE3E3E3"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -217,55 +245,33 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFE3E3E3"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,118 +587,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81820F55-57B8-446B-A4A7-2EC74CDBEAFB}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="10"/>
-    <col min="11" max="11" width="27.5546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.21875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>10</v>
+      <c r="P1" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3">
-        <v>123</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6">
-        <v>37446</v>
-      </c>
+      <c r="C2" s="10">
+        <v>89302011953</v>
+      </c>
+      <c r="D2" s="8">
+        <v>123456789</v>
+      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6">
-        <v>45403</v>
-      </c>
-      <c r="I2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>12</v>
+      <c r="H2" s="9">
+        <v>32874</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="9">
+        <v>45292</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="H3" s="6"/>
-      <c r="K3" s="13"/>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="10">
+        <v>89302011953</v>
+      </c>
+      <c r="D3" s="4">
+        <v>987654321</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1">
+        <v>33636</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2">
+        <v>45323</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="H4" s="6"/>
-      <c r="K4" s="13"/>
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="10">
+        <v>89302011953</v>
+      </c>
+      <c r="D4" s="4">
+        <v>345678912</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1">
+        <v>31109</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2">
+        <v>45352</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H5"/>
-      <c r="J5"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="10">
+        <v>89302011953</v>
+      </c>
+      <c r="D5">
+        <v>789456123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2">
+        <v>32237</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="2">
+        <v>45383</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10">
+        <v>89302011953</v>
+      </c>
+      <c r="D6">
+        <v>921345678</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2">
+        <v>34824</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2">
+        <v>45413</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{3BBA6F20-EDC2-4EA7-9B6C-CCA8FE22D0A8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Disable input khi sách đã mượn(off) + lưu trạng thái thanh toán sau giao dịch VNPAy
</commit_message>
<xml_diff>
--- a/Library_API/Upload/importfile.xlsx
+++ b/Library_API/Upload/importfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK1 2024-2025\CT554 LuanVan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769E8FD3-A602-4CA7-921E-9E9195F53BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542EBAF4-C773-4398-91B5-334CB7C4534E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80549B35-C4EB-4A7C-B8D2-F0AF8A9BC7A4}"/>
+    <workbookView xWindow="4620" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{80549B35-C4EB-4A7C-B8D2-F0AF8A9BC7A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>HinhThe</t>
   </si>
   <si>
-    <t>apple_user</t>
-  </si>
-  <si>
     <t>pass123</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Ha Noi</t>
   </si>
   <si>
-    <t>banana_user</t>
-  </si>
-  <si>
     <t>pass456</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>Ho Chi Minh</t>
   </si>
   <si>
-    <t>cherry_user</t>
-  </si>
-  <si>
     <t>pass789</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>Da Nang</t>
   </si>
   <si>
-    <t>grape_user</t>
-  </si>
-  <si>
     <t>pass321</t>
   </si>
   <si>
@@ -144,9 +132,6 @@
     <t>Can Tho</t>
   </si>
   <si>
-    <t>mango_user</t>
-  </si>
-  <si>
     <t>pass654</t>
   </si>
   <si>
@@ -163,6 +148,21 @@
   </si>
   <si>
     <t>LoaiNguoiDung</t>
+  </si>
+  <si>
+    <t>apple_user1</t>
+  </si>
+  <si>
+    <t>banana_user1</t>
+  </si>
+  <si>
+    <t>cherry_user1</t>
+  </si>
+  <si>
+    <t>grape_user1</t>
+  </si>
+  <si>
+    <t>mango_user1</t>
   </si>
 </sst>
 </file>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81820F55-57B8-446B-A4A7-2EC74CDBEAFB}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s">
         <v>7</v>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -662,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C2" s="10">
         <v>89302011953</v>
@@ -672,22 +672,22 @@
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="H2" s="9">
         <v>32874</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="L2" s="9">
         <v>45292</v>
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C3" s="10">
         <v>89302011953</v>
@@ -717,22 +717,22 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1">
         <v>33636</v>
       </c>
       <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="L3" s="2">
         <v>45323</v>
@@ -752,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C4" s="10">
         <v>89302011953</v>
@@ -762,22 +762,22 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1">
         <v>31109</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2">
         <v>45352</v>
@@ -797,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C5" s="10">
         <v>89302011953</v>
@@ -806,22 +806,22 @@
         <v>789456123</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2">
         <v>32237</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L5" s="2">
         <v>45383</v>
@@ -841,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10">
         <v>89302011953</v>
@@ -850,22 +850,22 @@
         <v>921345678</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H6" s="2">
         <v>34824</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L6" s="2">
         <v>45413</v>

</xml_diff>